<commit_message>
add mono mast3r & fix scale estimation
</commit_message>
<xml_diff>
--- a/full_evaluation_results_s1.0.xlsx
+++ b/full_evaluation_results_s1.0.xlsx
@@ -517,22 +517,22 @@
         <v>4.473532199859619</v>
       </c>
       <c r="G2" t="n">
-        <v>59.56562423706055</v>
+        <v>108.6829299926758</v>
       </c>
       <c r="H2" t="n">
-        <v>164.8483581542969</v>
+        <v>317.6914978027344</v>
       </c>
       <c r="I2" t="n">
-        <v>1.463595986366272</v>
+        <v>3.086787939071655</v>
       </c>
       <c r="J2" t="n">
-        <v>8.259799957275391</v>
+        <v>10.21835327148438</v>
       </c>
       <c r="K2" t="n">
-        <v>0.764115311665241</v>
+        <v>0.430992442154261</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8938075178093381</v>
+        <v>1.990642279791056</v>
       </c>
     </row>
     <row r="3">
@@ -557,22 +557,22 @@
         <v>2.812749147415161</v>
       </c>
       <c r="G3" t="n">
-        <v>81.57760620117188</v>
+        <v>99.13406372070312</v>
       </c>
       <c r="H3" t="n">
-        <v>168.5567169189453</v>
+        <v>216.0992126464844</v>
       </c>
       <c r="I3" t="n">
-        <v>4.688079833984375</v>
+        <v>6.81588077545166</v>
       </c>
       <c r="J3" t="n">
-        <v>5.651810169219971</v>
+        <v>6.334219932556152</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1438250380290623</v>
+        <v>0.08980409620695536</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8707856019194653</v>
+        <v>1.259197856155351</v>
       </c>
     </row>
     <row r="4">
@@ -597,22 +597,22 @@
         <v>3.796956777572632</v>
       </c>
       <c r="G4" t="n">
-        <v>68.68374633789062</v>
+        <v>165.6681060791016</v>
       </c>
       <c r="H4" t="n">
-        <v>209.6996154785156</v>
+        <v>740.0010986328125</v>
       </c>
       <c r="I4" t="n">
-        <v>3.625239372253418</v>
+        <v>7.536784648895264</v>
       </c>
       <c r="J4" t="n">
-        <v>9.021976470947266</v>
+        <v>16.80570793151855</v>
       </c>
       <c r="K4" t="n">
-        <v>2.638785086827506</v>
+        <v>3.225817004402545</v>
       </c>
       <c r="L4" t="n">
-        <v>3.130476523792711</v>
+        <v>6.791158183206554</v>
       </c>
     </row>
     <row r="5">
@@ -677,22 +677,22 @@
         <v>3.260169982910156</v>
       </c>
       <c r="G6" t="n">
-        <v>80.47314453125</v>
+        <v>73.77909851074219</v>
       </c>
       <c r="H6" t="n">
-        <v>275.4366149902344</v>
+        <v>273.7779846191406</v>
       </c>
       <c r="I6" t="n">
-        <v>2.029704332351685</v>
+        <v>2.889680862426758</v>
       </c>
       <c r="J6" t="n">
-        <v>9.55146598815918</v>
+        <v>9.387054443359375</v>
       </c>
       <c r="K6" t="n">
-        <v>0.7893062114370805</v>
+        <v>0.4648379908907747</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8619251753941057</v>
+        <v>1.229267315286151</v>
       </c>
     </row>
     <row r="7">
@@ -757,22 +757,22 @@
         <v>3.979043245315552</v>
       </c>
       <c r="G8" t="n">
-        <v>196.1536102294922</v>
+        <v>116.0167922973633</v>
       </c>
       <c r="H8" t="n">
-        <v>1011.827941894531</v>
+        <v>435.6024169921875</v>
       </c>
       <c r="I8" t="n">
-        <v>12.51039409637451</v>
+        <v>5.029820442199707</v>
       </c>
       <c r="J8" t="n">
-        <v>31.42294883728027</v>
+        <v>20.85674095153809</v>
       </c>
       <c r="K8" t="n">
-        <v>1.281190600680846</v>
+        <v>0.5089652009826994</v>
       </c>
       <c r="L8" t="n">
-        <v>4.674372602373738</v>
+        <v>1.983294202847733</v>
       </c>
     </row>
     <row r="9">
@@ -797,22 +797,22 @@
         <v>4.539266586303711</v>
       </c>
       <c r="G9" t="n">
-        <v>150.1956176757812</v>
+        <v>166.8375091552734</v>
       </c>
       <c r="H9" t="n">
-        <v>396.3038024902344</v>
+        <v>443.2389831542969</v>
       </c>
       <c r="I9" t="n">
-        <v>4.452651023864746</v>
+        <v>4.949410438537598</v>
       </c>
       <c r="J9" t="n">
-        <v>15.90319633483887</v>
+        <v>16.43637275695801</v>
       </c>
       <c r="K9" t="n">
-        <v>1.097454258268168</v>
+        <v>1.317884681673736</v>
       </c>
       <c r="L9" t="n">
-        <v>1.370247607276749</v>
+        <v>1.501406740404275</v>
       </c>
     </row>
     <row r="10">
@@ -837,22 +837,22 @@
         <v>3.431593179702759</v>
       </c>
       <c r="G10" t="n">
-        <v>97.97261810302734</v>
+        <v>47.57673645019531</v>
       </c>
       <c r="H10" t="n">
-        <v>271.9375305175781</v>
+        <v>113.9475021362305</v>
       </c>
       <c r="I10" t="n">
-        <v>2.589782953262329</v>
+        <v>0.3832592964172363</v>
       </c>
       <c r="J10" t="n">
-        <v>9.677444458007812</v>
+        <v>8.047077178955078</v>
       </c>
       <c r="K10" t="n">
-        <v>0.7660528676468703</v>
+        <v>0.08098722138961886</v>
       </c>
       <c r="L10" t="n">
-        <v>0.7614479712342376</v>
+        <v>0.1102630363814392</v>
       </c>
     </row>
     <row r="11">
@@ -917,22 +917,22 @@
         <v>5.822107315063477</v>
       </c>
       <c r="G12" t="n">
-        <v>65.13388061523438</v>
+        <v>57.89563751220703</v>
       </c>
       <c r="H12" t="n">
-        <v>153.0772247314453</v>
+        <v>155.9514923095703</v>
       </c>
       <c r="I12" t="n">
-        <v>0.4819254279136658</v>
+        <v>0.2485483884811401</v>
       </c>
       <c r="J12" t="n">
-        <v>13.58760452270508</v>
+        <v>13.51173210144043</v>
       </c>
       <c r="K12" t="n">
-        <v>0.07854345985623039</v>
+        <v>0.03533377400280525</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1164748693354014</v>
+        <v>0.03621065308990438</v>
       </c>
     </row>
     <row r="13">
@@ -997,22 +997,22 @@
         <v>4.987997531890869</v>
       </c>
       <c r="G14" t="n">
-        <v>302.9744567871094</v>
+        <v>249.5182952880859</v>
       </c>
       <c r="H14" t="n">
-        <v>771.2894897460938</v>
+        <v>668.255615234375</v>
       </c>
       <c r="I14" t="n">
-        <v>8.797893524169922</v>
+        <v>7.366587162017822</v>
       </c>
       <c r="J14" t="n">
-        <v>16.84098625183105</v>
+        <v>14.78339099884033</v>
       </c>
       <c r="K14" t="n">
-        <v>4.97494919657057</v>
+        <v>3.614055647838236</v>
       </c>
       <c r="L14" t="n">
-        <v>5.289371235980503</v>
+        <v>4.433842816713573</v>
       </c>
     </row>
     <row r="15">
@@ -1037,22 +1037,22 @@
         <v>3.71514368057251</v>
       </c>
       <c r="G15" t="n">
-        <v>149.8555603027344</v>
+        <v>124.0782470703125</v>
       </c>
       <c r="H15" t="n">
-        <v>285.263916015625</v>
+        <v>227.3143310546875</v>
       </c>
       <c r="I15" t="n">
-        <v>6.356755256652832</v>
+        <v>4.94888162612915</v>
       </c>
       <c r="J15" t="n">
-        <v>8.786289215087891</v>
+        <v>7.703754425048828</v>
       </c>
       <c r="K15" t="n">
-        <v>0.2093348215173136</v>
+        <v>0.1348285218486699</v>
       </c>
       <c r="L15" t="n">
-        <v>1.03737121748157</v>
+        <v>0.7558165751667402</v>
       </c>
     </row>
     <row r="16">
@@ -1077,22 +1077,22 @@
         <v>5.023480415344238</v>
       </c>
       <c r="G16" t="n">
-        <v>75.48699951171875</v>
+        <v>79.10270690917969</v>
       </c>
       <c r="H16" t="n">
-        <v>239.5101318359375</v>
+        <v>245.5284118652344</v>
       </c>
       <c r="I16" t="n">
-        <v>1.305710792541504</v>
+        <v>0.9533370137214661</v>
       </c>
       <c r="J16" t="n">
-        <v>8.370334625244141</v>
+        <v>8.215726852416992</v>
       </c>
       <c r="K16" t="n">
-        <v>0.6302772025502184</v>
+        <v>0.5461294901259565</v>
       </c>
       <c r="L16" t="n">
-        <v>0.8475301852201448</v>
+        <v>0.610382169987709</v>
       </c>
     </row>
     <row r="17">
@@ -1117,22 +1117,22 @@
         <v>7.062256813049316</v>
       </c>
       <c r="G17" t="n">
-        <v>133.7837677001953</v>
+        <v>115.2895736694336</v>
       </c>
       <c r="H17" t="n">
-        <v>375.4980163574219</v>
+        <v>317.4119262695312</v>
       </c>
       <c r="I17" t="n">
-        <v>2.07244610786438</v>
+        <v>1.091237187385559</v>
       </c>
       <c r="J17" t="n">
-        <v>13.47560119628906</v>
+        <v>13.26593208312988</v>
       </c>
       <c r="K17" t="n">
-        <v>0.4832464818160446</v>
+        <v>0.3075736701257018</v>
       </c>
       <c r="L17" t="n">
-        <v>0.7702279171783946</v>
+        <v>0.388819887458323</v>
       </c>
     </row>
     <row r="18">
@@ -1157,22 +1157,22 @@
         <v>4.666821479797363</v>
       </c>
       <c r="G18" t="n">
-        <v>111.4621963500977</v>
+        <v>90.23635864257812</v>
       </c>
       <c r="H18" t="n">
-        <v>239.3534240722656</v>
+        <v>187.8910522460938</v>
       </c>
       <c r="I18" t="n">
-        <v>1.626081824302673</v>
+        <v>0.8822309970855713</v>
       </c>
       <c r="J18" t="n">
-        <v>10.0245418548584</v>
+        <v>9.339920043945312</v>
       </c>
       <c r="K18" t="n">
-        <v>0.2674947771974942</v>
+        <v>0.1272548079570197</v>
       </c>
       <c r="L18" t="n">
-        <v>0.5612240171114848</v>
+        <v>0.2722432278784981</v>
       </c>
     </row>
     <row r="19">
@@ -1197,22 +1197,22 @@
         <v>7.309549808502197</v>
       </c>
       <c r="G19" t="n">
-        <v>176.8385925292969</v>
+        <v>125.7876358032227</v>
       </c>
       <c r="H19" t="n">
-        <v>551.8920288085938</v>
+        <v>521.701171875</v>
       </c>
       <c r="I19" t="n">
-        <v>4.476409912109375</v>
+        <v>5.127596855163574</v>
       </c>
       <c r="J19" t="n">
-        <v>15.38296794891357</v>
+        <v>17.47074127197266</v>
       </c>
       <c r="K19" t="n">
-        <v>2.05796257626427</v>
+        <v>0.6956230466389091</v>
       </c>
       <c r="L19" t="n">
-        <v>2.107067469067945</v>
+        <v>2.540412812436776</v>
       </c>
     </row>
     <row r="20">
@@ -1277,22 +1277,22 @@
         <v>5.481054306030273</v>
       </c>
       <c r="G21" t="n">
-        <v>104.2088623046875</v>
+        <v>137.5004425048828</v>
       </c>
       <c r="H21" t="n">
-        <v>322.9708557128906</v>
+        <v>408.0429382324219</v>
       </c>
       <c r="I21" t="n">
-        <v>1.517764687538147</v>
+        <v>2.171093463897705</v>
       </c>
       <c r="J21" t="n">
-        <v>8.479915618896484</v>
+        <v>9.779004096984863</v>
       </c>
       <c r="K21" t="n">
-        <v>0.4886878092413954</v>
+        <v>0.8812014897652418</v>
       </c>
       <c r="L21" t="n">
-        <v>0.8184771003386079</v>
+        <v>1.230758937724136</v>
       </c>
     </row>
     <row r="22">
@@ -1357,22 +1357,22 @@
         <v>4.637044429779053</v>
       </c>
       <c r="G23" t="n">
-        <v>83.91310882568359</v>
+        <v>77.65883636474609</v>
       </c>
       <c r="H23" t="n">
-        <v>200.92138671875</v>
+        <v>184.5671997070312</v>
       </c>
       <c r="I23" t="n">
-        <v>1.233413696289062</v>
+        <v>1.013454437255859</v>
       </c>
       <c r="J23" t="n">
-        <v>9.086774826049805</v>
+        <v>9.039108276367188</v>
       </c>
       <c r="K23" t="n">
-        <v>0.1772030503372498</v>
+        <v>0.1385385312536891</v>
       </c>
       <c r="L23" t="n">
-        <v>0.2151990588817293</v>
+        <v>0.166911543036723</v>
       </c>
     </row>
     <row r="24">
@@ -1397,22 +1397,22 @@
         <v>5.207028388977051</v>
       </c>
       <c r="G24" t="n">
-        <v>115.7272033691406</v>
+        <v>88.29719543457031</v>
       </c>
       <c r="H24" t="n">
-        <v>326.2965087890625</v>
+        <v>237.0995788574219</v>
       </c>
       <c r="I24" t="n">
-        <v>1.2666255235672</v>
+        <v>0.79860520362854</v>
       </c>
       <c r="J24" t="n">
-        <v>13.70786666870117</v>
+        <v>13.37563800811768</v>
       </c>
       <c r="K24" t="n">
-        <v>0.2712173280396838</v>
+        <v>0.1596388178446454</v>
       </c>
       <c r="L24" t="n">
-        <v>0.3537802603583006</v>
+        <v>0.1775355738014216</v>
       </c>
     </row>
     <row r="25">
@@ -1437,22 +1437,22 @@
         <v>4.915863513946533</v>
       </c>
       <c r="G25" t="n">
-        <v>50.04081726074219</v>
+        <v>56.22836303710938</v>
       </c>
       <c r="H25" t="n">
-        <v>188.8284149169922</v>
+        <v>210.8364410400391</v>
       </c>
       <c r="I25" t="n">
-        <v>0.8170096874237061</v>
+        <v>0.709577739238739</v>
       </c>
       <c r="J25" t="n">
-        <v>10.37972545623779</v>
+        <v>10.7540111541748</v>
       </c>
       <c r="K25" t="n">
-        <v>0.3227047162238519</v>
+        <v>0.2740642153934587</v>
       </c>
       <c r="L25" t="n">
-        <v>0.6888003602467576</v>
+        <v>0.6239872640883656</v>
       </c>
     </row>
     <row r="26">
@@ -1515,22 +1515,22 @@
         <v>4.664289474487305</v>
       </c>
       <c r="G27" t="n">
-        <v>133.2182006835938</v>
+        <v>133.3283081054688</v>
       </c>
       <c r="H27" t="n">
-        <v>402.9666748046875</v>
+        <v>416.593017578125</v>
       </c>
       <c r="I27" t="n">
-        <v>4.07021427154541</v>
+        <v>4.061065196990967</v>
       </c>
       <c r="J27" t="n">
-        <v>12.38776874542236</v>
+        <v>12.60750770568848</v>
       </c>
       <c r="K27" t="n">
-        <v>1.067102966307782</v>
+        <v>0.8907501605608155</v>
       </c>
       <c r="L27" t="n">
-        <v>2.143088024854634</v>
+        <v>2.172430600232776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>